<commit_message>
added conjtrols to select file. read. clear.
</commit_message>
<xml_diff>
--- a/Mir/External/testdata/manual_edited.xlsx
+++ b/Mir/External/testdata/manual_edited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35850\Desktop\repositories\learning2\Learning\Mir\External\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6533BD79-61D6-4C73-A6F7-2E44CC03D755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A742D6-3512-4E30-B2C1-1B350A8E30BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="68">
   <si>
     <t>READY TO START
 FOR EXTERNAL 
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>DigitalOutput05</t>
-  </si>
-  <si>
-    <t>DigitalOutput06</t>
   </si>
   <si>
     <t>NAOH
@@ -594,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,19 +604,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -630,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -647,7 +644,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -664,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -681,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -698,7 +695,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -708,17 +705,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" t="s">
         <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -729,16 +717,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -746,16 +734,16 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -763,16 +751,16 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -780,16 +768,16 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -797,16 +785,16 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -814,16 +802,16 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -831,16 +819,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -848,16 +836,16 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
         <v>28</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -865,13 +853,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
@@ -882,16 +870,16 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -899,16 +887,16 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,13 +904,13 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
@@ -933,13 +921,13 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
@@ -950,13 +938,13 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -967,13 +955,13 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -984,13 +972,13 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
@@ -1001,16 +989,16 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,16 +1006,16 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1035,13 +1023,13 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1052,16 +1040,16 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
         <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1069,16 +1057,16 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1086,16 +1074,16 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1103,16 +1091,16 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1120,16 +1108,16 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,16 +1125,16 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,16 +1142,16 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1171,16 +1159,16 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,16 +1176,16 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1205,13 +1193,13 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
@@ -1222,13 +1210,13 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
         <v>44</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>45</v>
       </c>
       <c r="E37" t="s">
         <v>1</v>
@@ -1239,13 +1227,13 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
         <v>55</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>56</v>
       </c>
       <c r="E38" t="s">
         <v>1</v>
@@ -1256,16 +1244,16 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" t="s">
         <v>55</v>
       </c>
-      <c r="C39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>56</v>
-      </c>
-      <c r="E39" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1273,13 +1261,13 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
         <v>55</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>56</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
@@ -1290,13 +1278,13 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
         <v>1</v>
@@ -1307,13 +1295,13 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
@@ -1324,13 +1312,13 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
         <v>1</v>

</xml_diff>